<commit_message>
yank debug prints from tools_xl.py
</commit_message>
<xml_diff>
--- a/amanzi/aqua/xl/test.xlsx
+++ b/amanzi/aqua/xl/test.xlsx
@@ -7,26 +7,18 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="requirements - PASS" sheetId="1" r:id="rId1"/>
-    <sheet name="requirements - FAIL" sheetId="2" r:id="rId2"/>
-    <sheet name="requirements - NULL" sheetId="3" r:id="rId3"/>
-    <sheet name="provenance" sheetId="4" r:id="rId4"/>
+    <sheet name="provenance" sheetId="1" r:id="rId1"/>
+    <sheet name="requirements - PASS" sheetId="2" r:id="rId2"/>
+    <sheet name="requirements - FAIL" sheetId="3" r:id="rId3"/>
+    <sheet name="requirements - NULL" sheetId="4" r:id="rId4"/>
+    <sheet name="08-BC" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>Summary of requirements PASSED</t>
-  </si>
-  <si>
-    <t>Summary of requirements FAIL</t>
-  </si>
-  <si>
-    <t>Summary of requirements NULL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>AMANZI: The Multi-Process HPC Simulator</t>
   </si>
@@ -37,7 +29,7 @@
     <t>python source</t>
   </si>
   <si>
-    <t>echo.pyc</t>
+    <t>tools_xl.py</t>
   </si>
   <si>
     <t>directory</t>
@@ -99,6 +91,18 @@
   </si>
   <si>
     <t>operating systems</t>
+  </si>
+  <si>
+    <t>Summary or requirements PASSED</t>
+  </si>
+  <si>
+    <t>Summary or requirements FAIL</t>
+  </si>
+  <si>
+    <t>Summary or requirements NULL</t>
+  </si>
+  <si>
+    <t>08-Boundary Conditions</t>
   </si>
 </sst>
 </file>
@@ -117,19 +121,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,15 +155,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -456,81 +460,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;L&amp;8&amp;T
-&amp;8&amp;D&amp;C &amp;P / &amp;N&amp;R&amp;8&amp;Z
-&amp;8&amp;F</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;L&amp;8&amp;T
-&amp;8&amp;D&amp;C &amp;P / &amp;N&amp;R&amp;8&amp;Z
-&amp;8&amp;F</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;L&amp;8&amp;T
-&amp;8&amp;D&amp;C &amp;P / &amp;N&amp;R&amp;8&amp;Z
-&amp;8&amp;F</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -539,84 +471,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
+      <c r="A3" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
+      <c r="A8" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3">
-        <v>43434.83528628493</v>
+        <v>43434.8592612651</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="1" t="s">
-        <v>19</v>
+      <c r="A14" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <f> INFO( "system" )</f>
@@ -625,7 +557,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <f> INFO( "recalc" )</f>
@@ -634,7 +566,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <f> INFO( "numfile" )</f>
@@ -643,7 +575,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <f> INFO( "origin" )</f>
@@ -652,7 +584,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <f> INFO( "release" )</f>
@@ -661,7 +593,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <f> INFO( "directory" )</f>
@@ -670,7 +602,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <f> INFO( "osversion" )</f>
@@ -689,4 +621,100 @@
 &amp;8&amp;F</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;L&amp;8&amp;T
+&amp;8&amp;D&amp;C &amp;P / &amp;N&amp;R&amp;8&amp;Z
+&amp;8&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;L&amp;8&amp;T
+&amp;8&amp;D&amp;C &amp;P / &amp;N&amp;R&amp;8&amp;Z
+&amp;8&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;L&amp;8&amp;T
+&amp;8&amp;D&amp;C &amp;P / &amp;N&amp;R&amp;8&amp;Z
+&amp;8&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;L&amp;8&amp;T
+&amp;8&amp;D&amp;C &amp;P / &amp;N&amp;R&amp;8&amp;Z
+&amp;8&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
trying to loop over chapter sections
</commit_message>
<xml_diff>
--- a/amanzi/aqua/xl/test.xlsx
+++ b/amanzi/aqua/xl/test.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>AMANZI: The Multi-Process HPC Simulator</t>
   </si>
@@ -29,7 +29,7 @@
     <t>python source</t>
   </si>
   <si>
-    <t>tools_xl.py</t>
+    <t>tools_xl.pyc</t>
   </si>
   <si>
     <t>directory</t>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>08-Boundary Conditions</t>
+  </si>
+  <si>
+    <t>08-BC</t>
   </si>
 </sst>
 </file>
@@ -538,7 +541,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="3">
-        <v>43434.8592612651</v>
+        <v>43434.86570732237</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -697,7 +700,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -706,6 +709,11 @@
     <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sec key working at level 1
</commit_message>
<xml_diff>
--- a/amanzi/aqua/xl/test.xlsx
+++ b/amanzi/aqua/xl/test.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>AMANZI: The Multi-Process HPC Simulator</t>
   </si>
@@ -105,7 +105,13 @@
     <t>08-Boundary Conditions</t>
   </si>
   <si>
-    <t>08-BC</t>
+    <t>08-BC.S-01</t>
+  </si>
+  <si>
+    <t>08-BC.S-02</t>
+  </si>
+  <si>
+    <t>08-BC.S-03</t>
   </si>
 </sst>
 </file>
@@ -541,7 +547,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="3">
-        <v>43434.87062537717</v>
+        <v>43435.42160976339</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -713,7 +719,7 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Posting sections to XL
</commit_message>
<xml_diff>
--- a/amanzi/aqua/xl/test.xlsx
+++ b/amanzi/aqua/xl/test.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>AMANZI: The Multi-Process HPC Simulator</t>
   </si>
@@ -108,10 +108,19 @@
     <t>08-BC.S-01</t>
   </si>
   <si>
+    <t>assigned_region</t>
+  </si>
+  <si>
     <t>08-BC.S-02</t>
   </si>
   <si>
+    <t>liquid_phase</t>
+  </si>
+  <si>
     <t>08-BC.S-03</t>
+  </si>
+  <si>
+    <t>solid_phase</t>
   </si>
 </sst>
 </file>
@@ -547,7 +556,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="3">
-        <v>43435.42160976339</v>
+        <v>43435.44090384839</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -706,20 +715,42 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recursion - baby steps
</commit_message>
<xml_diff>
--- a/amanzi/aqua/xl/test.xlsx
+++ b/amanzi/aqua/xl/test.xlsx
@@ -108,19 +108,19 @@
     <t>08-BC.S-01</t>
   </si>
   <si>
-    <t>assigned_region</t>
+    <t>1. assigned_region</t>
   </si>
   <si>
     <t>08-BC.S-02</t>
   </si>
   <si>
-    <t>liquid_phase</t>
+    <t>2. liquid_phase</t>
   </si>
   <si>
     <t>08-BC.S-03</t>
   </si>
   <si>
-    <t>solid_phase</t>
+    <t>3. solid_phase</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="3">
-        <v>43435.44090384839</v>
+        <v>43435.51472035676</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -722,6 +722,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
point to output file
</commit_message>
<xml_diff>
--- a/amanzi/aqua/xl/test.xlsx
+++ b/amanzi/aqua/xl/test.xlsx
@@ -29,20 +29,20 @@
     <t>python source</t>
   </si>
   <si>
-    <t>tools_xl.pyc</t>
+    <t>tools_xl.py</t>
   </si>
   <si>
     <t>directory</t>
   </si>
   <si>
-    <t>/Users/dantopa/Documents/repos/GitHub/topa-development/amanzi/aqua/xl</t>
+    <t>/Volumes/Tlaltecuhtli/repos/GitHub/topa-development/amanzi/aqua/xl</t>
   </si>
   <si>
     <t>python version</t>
   </si>
   <si>
-    <t>2.7.10 (default, Jul 15 2017, 17:16:57) 
-[GCC 4.2.1 Compatible Apple LLVM 9.0.0 (clang-900.0.31)]</t>
+    <t>3.7.0 (default, Jun 28 2018, 07:39:16) 
+[Clang 4.0.1 (tags/RELEASE_401/final)]</t>
   </si>
   <si>
     <t>Environment variables</t>
@@ -51,19 +51,19 @@
     <t>$USER</t>
   </si>
   <si>
-    <t>dantopa</t>
+    <t>l127914</t>
   </si>
   <si>
     <t>$HOSTNAME</t>
   </si>
   <si>
-    <t>MacBookPro11,3</t>
+    <t>Cauchy.Schwarz</t>
   </si>
   <si>
     <t>$HOME</t>
   </si>
   <si>
-    <t>/Users/dantopa</t>
+    <t>/Users/l127914</t>
   </si>
   <si>
     <t>timestamp</t>
@@ -108,19 +108,19 @@
     <t>08-BC.S-01</t>
   </si>
   <si>
-    <t>1. assigned_region</t>
+    <t>1.assigned_region</t>
   </si>
   <si>
     <t>08-BC.S-02</t>
   </si>
   <si>
-    <t>2. liquid_phase</t>
+    <t>2.liquid_phase</t>
   </si>
   <si>
     <t>08-BC.S-03</t>
   </si>
   <si>
-    <t>3. solid_phase</t>
+    <t>3.solid_phase</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="3">
-        <v>43435.51472035676</v>
+        <v>43437.44765421725</v>
       </c>
     </row>
     <row r="14" spans="1:2">

</xml_diff>